<commit_message>
editing in test data and regression suite
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{633DF238-9F41-4049-B1CD-BC4CBB27DD1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{416F33BD-2220-4879-8CA5-103B05093771}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="7660" windowHeight="11060" activeTab="1" xr2:uid="{AAC25BE3-86A4-4DF6-B1E6-A276AEAFAAB1}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="7740" windowHeight="11060" activeTab="1" xr2:uid="{AAC25BE3-86A4-4DF6-B1E6-A276AEAFAAB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
     <sheet name="RegisterTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J11"/>
+  <oleSize ref="A1:E3"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>Nada_0987</t>
-  </si>
-  <si>
     <t>nadasalama9@gmail.com</t>
   </si>
   <si>
@@ -69,7 +66,10 @@
     <t>ALias is here</t>
   </si>
   <si>
-    <t>nadasalama5@gmail.com</t>
+    <t>Nada_1234</t>
+  </si>
+  <si>
+    <t>nadasalama4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE62B3A0-D83A-4797-9C29-11A538E56A97}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -445,10 +447,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -468,7 +470,7 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,43 +496,43 @@
         <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>